<commit_message>
Updated converter unit tests.
</commit_message>
<xml_diff>
--- a/tass-converter/tests/data/simple_demo.xlsx
+++ b/tass-converter/tests/data/simple_demo.xlsx
@@ -1,25 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desjajo\Documents\_TASS\tass-ssat-framework\tass-ssat\tass-converter\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735DE049-C8E8-4B13-B241-E99CD6E36F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{735DE049-C8E8-4B13-B241-E99CD6E36F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0818397A-86FC-48EB-99AE-E4977BBE10AC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tr0001" sheetId="1" r:id="rId1"/>
-    <sheet name="rTestrail" sheetId="4" r:id="rId2"/>
-    <sheet name="tc0001" sheetId="2" r:id="rId3"/>
-    <sheet name="tc0002" sheetId="3" r:id="rId4"/>
+    <sheet name="chrome001" sheetId="5" r:id="rId2"/>
+    <sheet name="rTestrail" sheetId="4" r:id="rId3"/>
+    <sheet name="tc0001" sheetId="2" r:id="rId4"/>
+    <sheet name="tc0002" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -28,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="84">
   <si>
     <t>tr_uuid:</t>
   </si>
@@ -36,6 +51,12 @@
     <t>tr100101</t>
   </si>
   <si>
+    <t>title:</t>
+  </si>
+  <si>
+    <t>sample-run</t>
+  </si>
+  <si>
     <t>build:</t>
   </si>
   <si>
@@ -51,15 +72,108 @@
     <t>uuid-tc-01</t>
   </si>
   <si>
+    <t>reporters:</t>
+  </si>
+  <si>
+    <t>testrail-1</t>
+  </si>
+  <si>
+    <t>browsers:</t>
+  </si>
+  <si>
+    <t>chrome001</t>
+  </si>
+  <si>
+    <t>other:</t>
+  </si>
+  <si>
+    <t>testrail</t>
+  </si>
+  <si>
     <t>Uuid-tc-02</t>
   </si>
   <si>
+    <t>project_id,321</t>
+  </si>
+  <si>
+    <t>br_uuid:</t>
+  </si>
+  <si>
+    <t>browser_name:</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>key,value</t>
+  </si>
+  <si>
+    <t>flag</t>
+  </si>
+  <si>
+    <t>driver:</t>
+  </si>
+  <si>
+    <t>implicit_wait,5</t>
+  </si>
+  <si>
+    <t>browser_arguments:</t>
+  </si>
+  <si>
+    <t>--start-maximized</t>
+  </si>
+  <si>
+    <t>browser_preferences:</t>
+  </si>
+  <si>
+    <t>explicit_wait,10</t>
+  </si>
+  <si>
+    <t>r_uuid:</t>
+  </si>
+  <si>
+    <t>type:</t>
+  </si>
+  <si>
+    <t>mode:</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>connection:</t>
+  </si>
+  <si>
+    <t>user,~</t>
+  </si>
+  <si>
+    <t>config:</t>
+  </si>
+  <si>
+    <t>package:</t>
+  </si>
+  <si>
+    <t>tass.report.testrail</t>
+  </si>
+  <si>
+    <t>host,abc</t>
+  </si>
+  <si>
+    <t>class_name:</t>
+  </si>
+  <si>
+    <t>TassTestrailReporter</t>
+  </si>
+  <si>
+    <t>url-base,abc.123</t>
+  </si>
+  <si>
+    <t>ssl-verify,3</t>
+  </si>
+  <si>
     <t>tc_uuid:</t>
   </si>
   <si>
-    <t>title:</t>
-  </si>
-  <si>
     <t>Tass Sample Case A</t>
   </si>
   <si>
@@ -181,70 +295,13 @@
   </si>
   <si>
     <t>Tass Sample Case B</t>
-  </si>
-  <si>
-    <t>r_uuid:</t>
-  </si>
-  <si>
-    <t>testrail-1</t>
-  </si>
-  <si>
-    <t>type:</t>
-  </si>
-  <si>
-    <t>testrail</t>
-  </si>
-  <si>
-    <t>mode:</t>
-  </si>
-  <si>
-    <t>single</t>
-  </si>
-  <si>
-    <t>connection:</t>
-  </si>
-  <si>
-    <t>user,~</t>
-  </si>
-  <si>
-    <t>ssl-verify,3</t>
-  </si>
-  <si>
-    <t>package:</t>
-  </si>
-  <si>
-    <t>class_name:</t>
-  </si>
-  <si>
-    <t>config:</t>
-  </si>
-  <si>
-    <t>sample-run</t>
-  </si>
-  <si>
-    <t>other:</t>
-  </si>
-  <si>
-    <t>project_id,321</t>
-  </si>
-  <si>
-    <t>url-base,abc.123</t>
-  </si>
-  <si>
-    <t>host,abc</t>
-  </si>
-  <si>
-    <t>tass.report.testrail</t>
-  </si>
-  <si>
-    <t>TassTestrailReporter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -272,11 +329,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,15 +649,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.6"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,51 +665,63 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="H2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="D6" s="1"/>
     </row>
   </sheetData>
@@ -665,79 +735,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE08AD9-60B2-4F47-A615-E0C1ED754686}">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D22928-1B39-435D-9B75-7C5F08BC76C9}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.08984375" customWidth="1"/>
-    <col min="4" max="4" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>59</v>
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -746,6 +802,87 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE08AD9-60B2-4F47-A615-E0C1ED754686}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.6"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ10"/>
   <sheetViews>
@@ -753,205 +890,205 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1024" width="11.6328125" style="2"/>
+    <col min="1" max="1024" width="11.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="2" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="G7" s="3"/>
       <c r="I7" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="3" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="3" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -964,7 +1101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
@@ -972,241 +1109,241 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1024" width="11.6328125" style="2"/>
+    <col min="1" max="1024" width="11.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="2" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="G7" s="3"/>
       <c r="I7" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="3" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="G12" s="3"/>
       <c r="I12" s="2" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed locator issue. Added explicit maxsplit value for k/v pairs.
</commit_message>
<xml_diff>
--- a/tass-converter/tests/data/simple_demo.xlsx
+++ b/tass-converter/tests/data/simple_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desjajo\Documents\_TASS\tass-ssat-framework\tass-ssat\tass-converter\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{735DE049-C8E8-4B13-B241-E99CD6E36F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0818397A-86FC-48EB-99AE-E4977BBE10AC}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{735DE049-C8E8-4B13-B241-E99CD6E36F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BD2C35B-61F5-47CB-8AF7-3A24FE170485}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tr0001" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="85">
   <si>
     <t>tr_uuid:</t>
   </si>
@@ -240,61 +240,64 @@
     <t>selwait,wait_element_visible</t>
   </si>
   <si>
+    <t>xpath,//*[contains(@id, 'test')]</t>
+  </si>
+  <si>
+    <t>selenium,write</t>
+  </si>
+  <si>
+    <t>do a barrel roll</t>
+  </si>
+  <si>
+    <t>q4</t>
+  </si>
+  <si>
+    <t>Click a button</t>
+  </si>
+  <si>
+    <t>selenium,click</t>
+  </si>
+  <si>
+    <t>btnColor</t>
+  </si>
+  <si>
+    <t>q5</t>
+  </si>
+  <si>
+    <t>Read CSS</t>
+  </si>
+  <si>
+    <t>selenium,read_css</t>
+  </si>
+  <si>
+    <t>background-color</t>
+  </si>
+  <si>
+    <t>q6</t>
+  </si>
+  <si>
+    <t>Assert element is displayed</t>
+  </si>
+  <si>
+    <t>selenium,assert_displayed</t>
+  </si>
+  <si>
+    <t>btnX</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>q7</t>
+  </si>
+  <si>
+    <t>q8</t>
+  </si>
+  <si>
+    <t>Tass Sample Case B</t>
+  </si>
+  <si>
     <t>id,nameField</t>
-  </si>
-  <si>
-    <t>selenium,write</t>
-  </si>
-  <si>
-    <t>do a barrel roll</t>
-  </si>
-  <si>
-    <t>q4</t>
-  </si>
-  <si>
-    <t>Click a button</t>
-  </si>
-  <si>
-    <t>selenium,click</t>
-  </si>
-  <si>
-    <t>btnColor</t>
-  </si>
-  <si>
-    <t>q5</t>
-  </si>
-  <si>
-    <t>Read CSS</t>
-  </si>
-  <si>
-    <t>selenium,read_css</t>
-  </si>
-  <si>
-    <t>background-color</t>
-  </si>
-  <si>
-    <t>q6</t>
-  </si>
-  <si>
-    <t>Assert element is displayed</t>
-  </si>
-  <si>
-    <t>selenium,assert_displayed</t>
-  </si>
-  <si>
-    <t>btnX</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>q7</t>
-  </si>
-  <si>
-    <t>q8</t>
-  </si>
-  <si>
-    <t>Tass Sample Case B</t>
   </si>
 </sst>
 </file>
@@ -651,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.6"/>
@@ -886,13 +889,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.6"/>
   <cols>
-    <col min="1" max="1024" width="11.5703125" style="2"/>
+    <col min="1" max="3" width="11.5703125" style="2"/>
+    <col min="4" max="4" width="34" style="2" customWidth="1"/>
+    <col min="5" max="1024" width="11.5703125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1203,7 +1208,7 @@
         <v>64</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="2" t="s">
@@ -1296,7 +1301,7 @@
         <v>64</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2" t="s">

</xml_diff>

<commit_message>
Updated converter to accept new parameters.
</commit_message>
<xml_diff>
--- a/tass-converter/tests/data/simple_demo.xlsx
+++ b/tass-converter/tests/data/simple_demo.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desjajo\Documents\_Python\tass-ssat\tass-converter\tests\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9396C900-8324-4092-9E94-971C6B39F976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="tr0001" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="tr0002" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="tc0001" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="tc0002" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="chrome001" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="chrome002" sheetId="6" state="visible" r:id="rId8"/>
-    <sheet name="ffox001" sheetId="7" state="visible" r:id="rId9"/>
-    <sheet name="ffox002" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="tr0001" sheetId="1" r:id="rId1"/>
+    <sheet name="tr0002" sheetId="2" r:id="rId2"/>
+    <sheet name="tc0001" sheetId="3" r:id="rId3"/>
+    <sheet name="tc0002" sheetId="4" r:id="rId4"/>
+    <sheet name="chrome001" sheetId="5" r:id="rId5"/>
+    <sheet name="chrome002" sheetId="6" r:id="rId6"/>
+    <sheet name="ffox001" sheetId="7" r:id="rId7"/>
+    <sheet name="ffox002" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -27,263 +32,286 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="82">
-  <si>
-    <t xml:space="preserve">tr_uuid:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tr1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">build:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V2.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test suites:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test cases:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uuid-tc-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reporters:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">browsers:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chrome001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">others:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testrail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uuid-tc-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ffox002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project_id,321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tr2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chrome002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ffox001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tc_uuid:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tass Sample Case A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uuid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">main action</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">action</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relative_path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">attribute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">q1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Launch test page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selenium,load_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examples/demo-html/page1.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">q2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assert page is open</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selenium,assert_page_is_open</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sample,page1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">q3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wait for element then type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selwait,wait_element_visible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id,nameField</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selenium,write</t>
-  </si>
-  <si>
-    <t xml:space="preserve">do a barrel roll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">q4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click a button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selenium,click</t>
-  </si>
-  <si>
-    <t xml:space="preserve">btnColor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">q5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read CSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selenium,read_css</t>
-  </si>
-  <si>
-    <t xml:space="preserve">background-color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">q6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assert element is displayed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selenium,assert_displayed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">btnX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">q7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">q8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tass Sample Case B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locator_args</t>
-  </si>
-  <si>
-    <t xml:space="preserve">q6a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">btnFormat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">br_uuid:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">browser_name:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chrome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">key,value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">driver:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">implicit_wait,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">browser_arguments:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--start-maximized</t>
-  </si>
-  <si>
-    <t xml:space="preserve">browser_preferences:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">explicit_wait,10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">--headless</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firefox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">implicit_wait,15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">explicit_wait,30</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="91">
+  <si>
+    <t>tr_uuid:</t>
+  </si>
+  <si>
+    <t>tr1</t>
+  </si>
+  <si>
+    <t>title:</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>build:</t>
+  </si>
+  <si>
+    <t>V2.4</t>
+  </si>
+  <si>
+    <t>test suites:</t>
+  </si>
+  <si>
+    <t>test cases:</t>
+  </si>
+  <si>
+    <t>uuid-tc-01</t>
+  </si>
+  <si>
+    <t>reporters:</t>
+  </si>
+  <si>
+    <t>browsers:</t>
+  </si>
+  <si>
+    <t>chrome001</t>
+  </si>
+  <si>
+    <t>others:</t>
+  </si>
+  <si>
+    <t>testrail</t>
+  </si>
+  <si>
+    <t>Uuid-tc-02</t>
+  </si>
+  <si>
+    <t>ffox002</t>
+  </si>
+  <si>
+    <t>project_id,321</t>
+  </si>
+  <si>
+    <t>tr2</t>
+  </si>
+  <si>
+    <t>chrome002</t>
+  </si>
+  <si>
+    <t>ffox001</t>
+  </si>
+  <si>
+    <t>tc_uuid:</t>
+  </si>
+  <si>
+    <t>Tass Sample Case A</t>
+  </si>
+  <si>
+    <t>uuid</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>main action</t>
+  </si>
+  <si>
+    <t>locator</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>relative_path</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>soft</t>
+  </si>
+  <si>
+    <t>q1</t>
+  </si>
+  <si>
+    <t>Launch test page</t>
+  </si>
+  <si>
+    <t>selenium,load_file</t>
+  </si>
+  <si>
+    <t>examples/demo-html/page1.html</t>
+  </si>
+  <si>
+    <t>q2</t>
+  </si>
+  <si>
+    <t>Assert page is open</t>
+  </si>
+  <si>
+    <t>selenium,assert_page_is_open</t>
+  </si>
+  <si>
+    <t>sample,page1</t>
+  </si>
+  <si>
+    <t>q3</t>
+  </si>
+  <si>
+    <t>Wait for element then type</t>
+  </si>
+  <si>
+    <t>selwait,wait_element_visible</t>
+  </si>
+  <si>
+    <t>id,nameField</t>
+  </si>
+  <si>
+    <t>selenium,write</t>
+  </si>
+  <si>
+    <t>do a barrel roll</t>
+  </si>
+  <si>
+    <t>q4</t>
+  </si>
+  <si>
+    <t>Click a button</t>
+  </si>
+  <si>
+    <t>selenium,click</t>
+  </si>
+  <si>
+    <t>btnColor</t>
+  </si>
+  <si>
+    <t>q5</t>
+  </si>
+  <si>
+    <t>Read CSS</t>
+  </si>
+  <si>
+    <t>selenium,read_css</t>
+  </si>
+  <si>
+    <t>background-color</t>
+  </si>
+  <si>
+    <t>q6</t>
+  </si>
+  <si>
+    <t>Assert element is displayed</t>
+  </si>
+  <si>
+    <t>selenium,assert_displayed</t>
+  </si>
+  <si>
+    <t>btnX</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>q7</t>
+  </si>
+  <si>
+    <t>q8</t>
+  </si>
+  <si>
+    <t>Tass Sample Case B</t>
+  </si>
+  <si>
+    <t>locator_args</t>
+  </si>
+  <si>
+    <t>q6a</t>
+  </si>
+  <si>
+    <t>btnFormat</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>br_uuid:</t>
+  </si>
+  <si>
+    <t>browser_name:</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>key,value</t>
+  </si>
+  <si>
+    <t>flag</t>
+  </si>
+  <si>
+    <t>driver:</t>
+  </si>
+  <si>
+    <t>implicit_wait,5</t>
+  </si>
+  <si>
+    <t>browser_arguments:</t>
+  </si>
+  <si>
+    <t>--start-maximized</t>
+  </si>
+  <si>
+    <t>browser_preferences:</t>
+  </si>
+  <si>
+    <t>explicit_wait,10</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>--headless</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>implicit_wait,15</t>
+  </si>
+  <si>
+    <t>explicit_wait,30</t>
+  </si>
+  <si>
+    <t>q9</t>
+  </si>
+  <si>
+    <t>Click and drag</t>
+  </si>
+  <si>
+    <t>selchain,drag_and_drop</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>offset</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>id,btnX</t>
+  </si>
+  <si>
+    <t>10,20</t>
+  </si>
+  <si>
+    <t>100,90</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -291,25 +319,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF242424"/>
       <name val="Aptos Narrow"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -322,7 +334,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -330,65 +342,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -447,60 +418,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF242424"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -532,7 +519,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -556,7 +543,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -616,28 +603,27 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.71484375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -651,7 +637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -659,7 +645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -685,7 +671,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
@@ -696,12 +682,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -709,19 +693,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,7 +716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -743,7 +724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -769,7 +750,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
@@ -780,12 +761,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -793,26 +772,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="3" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="40.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="4" style="3" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="29.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="3" width="11.57"/>
+    <col min="1" max="2" width="11.5703125" style="3"/>
+    <col min="3" max="3" width="40.7109375" style="3" customWidth="1"/>
+    <col min="4" max="6" width="11.5703125" style="3"/>
+    <col min="7" max="7" width="29.5703125" style="3" customWidth="1"/>
+    <col min="8" max="1024" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -826,7 +802,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
@@ -857,8 +833,17 @@
       <c r="J2" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -874,7 +859,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
@@ -890,7 +875,7 @@
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>40</v>
       </c>
@@ -912,7 +897,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>46</v>
       </c>
@@ -930,7 +915,7 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
@@ -951,7 +936,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>54</v>
       </c>
@@ -971,7 +956,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>59</v>
       </c>
@@ -988,7 +973,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>60</v>
       </c>
@@ -1008,11 +993,36 @@
         <v>58</v>
       </c>
     </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1020,27 +1030,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AMJ13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="3" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="28.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="28.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="3" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="38.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="3" width="11.57"/>
+    <col min="1" max="2" width="11.5703125" style="3"/>
+    <col min="3" max="3" width="28.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="3" customWidth="1"/>
+    <col min="5" max="6" width="11.5703125" style="3"/>
+    <col min="7" max="7" width="38.85546875" style="3" customWidth="1"/>
+    <col min="8" max="1024" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -1054,7 +1061,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
@@ -1089,7 +1096,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -1105,7 +1112,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
@@ -1121,7 +1128,7 @@
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>40</v>
       </c>
@@ -1143,7 +1150,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>46</v>
       </c>
@@ -1161,7 +1168,7 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
@@ -1182,7 +1189,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
@@ -1198,7 +1205,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>36</v>
       </c>
@@ -1214,7 +1221,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>40</v>
       </c>
@@ -1236,7 +1243,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>46</v>
       </c>
@@ -1254,7 +1261,7 @@
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>50</v>
       </c>
@@ -1275,7 +1282,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>63</v>
       </c>
@@ -1297,10 +1304,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1308,26 +1314,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.42"/>
+    <col min="1" max="1" width="11.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>66</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>69</v>
       </c>
@@ -1352,7 +1355,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>71</v>
       </c>
@@ -1369,43 +1372,35 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.42"/>
+    <col min="1" max="1" width="11.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>66</v>
       </c>
@@ -1419,7 +1414,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>77</v>
       </c>
@@ -1430,7 +1425,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>71</v>
       </c>
@@ -1447,7 +1442,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>76</v>
       </c>
@@ -1456,37 +1451,29 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.42"/>
+    <col min="1" max="1" width="11.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>66</v>
       </c>
@@ -1500,7 +1487,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>69</v>
       </c>
@@ -1511,7 +1498,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>71</v>
       </c>
@@ -1528,43 +1515,35 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.42"/>
+    <col min="1" max="1" width="11.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>66</v>
       </c>
@@ -1578,7 +1557,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>69</v>
       </c>
@@ -1589,7 +1568,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>71</v>
       </c>
@@ -1604,18 +1583,13 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>